<commit_message>
Update: nre constraints (continuous charging)
</commit_message>
<xml_diff>
--- a/Instances/input_small.xlsx
+++ b/Instances/input_small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/UC/PhD/Math models/Electric Bus Smart Charging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/Electric Bus Smart Charging/Instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D91D5E-141D-6541-83A3-1B0B8CCD9820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F23A3C5-C8A5-2F41-A252-482B142B9CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31520" yWindow="2060" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
+    <workbookView xWindow="-31520" yWindow="1500" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -475,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B7F405-04BD-9A44-923D-D0B1D0915781}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,6 +501,11 @@
         <v>348</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -508,10 +513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC39ED6-C21E-184F-8399-91DE2859F8BB}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +548,16 @@
       </c>
       <c r="I2">
         <f>SUM(A2:A9)</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>D3/$F$2</f>
         <v>1.3333333333333333</v>
+      </c>
+      <c r="D3">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -556,7 +570,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,6 +616,20 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>CONVERT(E3,"hr","min")</f>
+        <v>360</v>
+      </c>
+      <c r="B3">
+        <f>CONVERT(F3,"hr","min")</f>
+        <v>1140</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="L3" s="1"/>
@@ -648,7 +676,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,11 +723,11 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>C2*$H$2</f>
-        <v>0.22030170399999999</v>
+        <v>0.17728832999999999</v>
       </c>
       <c r="C2">
         <f>D2+E2*F2*G2</f>
-        <v>1.1015085199999999</v>
+        <v>0.88644164999999997</v>
       </c>
       <c r="D2" s="4">
         <v>0.88644164999999997</v>
@@ -711,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f>12/60</f>
@@ -725,10 +753,26 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="A3">
+        <f>C3*$H$2</f>
+        <v>0.17728832999999999</v>
+      </c>
+      <c r="C3">
+        <f>D3+E3*F3*G3</f>
+        <v>0.88644164999999997</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.88644164999999997</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.21506686999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="4"/>
       <c r="L3" s="2"/>
@@ -13793,7 +13837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E9005A-C93F-D246-A03F-07B7DAAF214E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -13846,7 +13890,7 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B9" si="0">$D$3*F3</f>
+        <f t="shared" ref="B3" si="0">$D$3*F3</f>
         <v>4.3391999999999999</v>
       </c>
       <c r="C3">
@@ -13857,7 +13901,7 @@
         <v>2.1696</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F9" si="1">C3/80</f>
+        <f t="shared" ref="F3" si="1">C3/80</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Model working for continuous charging
</commit_message>
<xml_diff>
--- a/Instances/input_small.xlsx
+++ b/Instances/input_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/Electric Bus Smart Charging/Instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F23A3C5-C8A5-2F41-A252-482B142B9CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2864B4-2036-2642-91B3-18B2D86FF6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31520" yWindow="1500" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
+    <workbookView xWindow="-31520" yWindow="1500" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC39ED6-C21E-184F-8399-91DE2859F8BB}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -13837,8 +13837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E9005A-C93F-D246-A03F-07B7DAAF214E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
New Robust counterpart file
</commit_message>
<xml_diff>
--- a/Instances/input_small.xlsx
+++ b/Instances/input_small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/Electric Bus Smart Charging/Instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB0E044-A1A8-2C42-9331-4D85934D5E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6787B929-E4BC-4D4A-8A92-0BF27793C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17520" yWindow="1500" windowWidth="16240" windowHeight="18880" activeTab="3" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A9:XFD11"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,11 +723,11 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>C2*$H$2</f>
-        <v>0.17728832999999999</v>
+        <v>0.22030170399999999</v>
       </c>
       <c r="C2">
         <f>D2+E2*F2*G2</f>
-        <v>0.88644164999999997</v>
+        <v>1.1015085199999999</v>
       </c>
       <c r="D2" s="4">
         <v>0.88644164999999997</v>
@@ -739,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>12/60</f>
@@ -755,11 +755,11 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>C3*$H$2</f>
-        <v>0.17728832999999999</v>
+        <v>0.22030170399999999</v>
       </c>
       <c r="C3">
         <f>D3+E3*F3*G3</f>
-        <v>0.88644164999999997</v>
+        <v>1.1015085199999999</v>
       </c>
       <c r="D3" s="4">
         <v>0.88644164999999997</v>
@@ -771,10 +771,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4">
+        <f>E3*$H$2</f>
+        <v>4.3013374E-2</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -836,6 +839,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>